<commit_message>
补充数码管共阳信息 Signed-off-by: lecheng <lechenggood@foxmail.com>
</commit_message>
<xml_diff>
--- a/Hardware/v2.2 4HP/BOM_ContourLine2.2 4HP_ContourLine2.2 4HP_2024-07-29.xlsx
+++ b/Hardware/v2.2 4HP/BOM_ContourLine2.2 4HP_ContourLine2.2 4HP_2024-07-29.xlsx
@@ -645,7 +645,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">位数码管</t>
+      <t xml:space="preserve">位共阳数码管</t>
     </r>
   </si>
   <si>
@@ -1199,8 +1199,8 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1739,7 +1739,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>1</v>
       </c>

</xml_diff>